<commit_message>
save excel files for Quica and Leiva
</commit_message>
<xml_diff>
--- a/data/compiling/2023/CRCA/leiva/Cacao list-Katy & Frank-30 Dec 2023.xlsx
+++ b/data/compiling/2023/CRCA/leiva/Cacao list-Katy & Frank-30 Dec 2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frankjoyce/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francisjoyce/GitHub/ACG-CBC-data/data/compiling/2023/CRCA/leiva/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C032FA7B-6EF7-CA4C-B8A8-06905D338E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C235D778-47D3-F444-8D01-B341B1AE6603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="1540" windowWidth="28040" windowHeight="17200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="300" yWindow="1100" windowWidth="28040" windowHeight="17200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRCA_2023_updated_pre_cleaned" sheetId="1" r:id="rId1"/>
@@ -4626,7 +4626,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4649,7 +4649,6 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -4709,9 +4708,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4749,7 +4748,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -4855,7 +4854,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4997,7 +4996,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5007,7 +5006,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F507"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A481" zoomScale="128" zoomScaleNormal="128" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A319" zoomScale="128" zoomScaleNormal="128" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -7168,7 +7167,7 @@
       <c r="D158" s="7" t="s">
         <v>415</v>
       </c>
-      <c r="E158" s="14"/>
+      <c r="E158" s="8"/>
       <c r="F158" s="8"/>
     </row>
     <row r="159" spans="1:6" ht="34" x14ac:dyDescent="0.2">

</xml_diff>